<commit_message>
finish debug k_min, k_max
</commit_message>
<xml_diff>
--- a/output/strike grid & maturity grid recon.xlsx
+++ b/output/strike grid & maturity grid recon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Murex\Desktop\Local Vol Calibration\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\van92\OneDrive\Desktop\Local-Vol-Calibration\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{29541B96-960A-4767-A44E-2B6A80867C8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3D215AD-4F60-4CD3-B032-F6072ADCE736}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24D23CA-A0F5-4638-A303-EE4C1F1C8964}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="2985" windowWidth="18135" windowHeight="11355" xr2:uid="{EDE94B52-7784-4D5D-959F-34CE5F250930}"/>
+    <workbookView xWindow="-1095" yWindow="6780" windowWidth="23295" windowHeight="12930" xr2:uid="{EDE94B52-7784-4D5D-959F-34CE5F250930}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>vol</t>
   </si>
@@ -139,7 +139,28 @@
     <t>k (diff)</t>
   </si>
   <si>
-    <t>Price:</t>
+    <t>k_min</t>
+  </si>
+  <si>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>k_max</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>dk</t>
+  </si>
+  <si>
+    <t>Nk</t>
   </si>
 </sst>
 </file>
@@ -654,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F32581-4DE6-4154-B1B2-65CB32E50AF6}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,18 +688,62 @@
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="6" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1">
         <v>1.0822999976901</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1">
+        <v>0</v>
+      </c>
+      <c r="M1">
+        <v>5.3272499999999995E-4</v>
+      </c>
+      <c r="N1">
+        <v>1.065E-3</v>
+      </c>
+      <c r="O1">
+        <v>1.598E-3</v>
+      </c>
+      <c r="P1">
+        <v>2.1310000000000001E-3</v>
+      </c>
+      <c r="Q1">
+        <v>4.2620000000000002E-3</v>
+      </c>
+      <c r="R1">
+        <v>6.3930000000000002E-3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <f>N1-M1</f>
+        <v>5.3227500000000002E-4</v>
+      </c>
+      <c r="N2">
+        <f>O1-N1</f>
+        <v>5.3300000000000005E-4</v>
+      </c>
+      <c r="O2">
+        <f>P1-O1</f>
+        <v>5.3300000000000005E-4</v>
+      </c>
+      <c r="P2">
+        <f>Q1-P1</f>
+        <v>2.1310000000000001E-3</v>
+      </c>
+      <c r="Q2">
+        <f>R1-Q1</f>
+        <v>2.1310000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -690,22 +755,18 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
       <c r="H4" s="11" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>7</v>
       </c>
@@ -720,8 +781,18 @@
       <c r="G5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>-4.1106482744587503E-2</v>
+      </c>
+      <c r="I5">
+        <v>-4.1106446492200001E-2</v>
+      </c>
+      <c r="J5">
+        <f>I5-H5</f>
+        <v>3.6252387501656269E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
@@ -733,8 +804,21 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6">
+        <v>4.5297248358925103E-2</v>
+      </c>
+      <c r="I6">
+        <v>4.5297252020500001E-2</v>
+      </c>
+      <c r="J6">
+        <f>I6-H6</f>
+        <v>3.6615748974511142E-9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>10</v>
       </c>
@@ -746,16 +830,33 @@
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <f>H6-H5</f>
+        <v>8.6403731103512599E-2</v>
+      </c>
+      <c r="I7">
+        <f>I6-I5</f>
+        <v>8.6403698512699995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8">
+        <v>9.0951295898434399E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11" t="s">
         <v>1</v>
@@ -766,8 +867,15 @@
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9">
+        <f>H7/H8</f>
+        <v>94.999999999999915</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>5</v>
       </c>
@@ -781,7 +889,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
@@ -795,7 +903,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
@@ -809,7 +917,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -817,7 +925,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
@@ -837,7 +945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>0</v>
       </c>
@@ -857,7 +965,7 @@
         <v>0.1425855308592</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>2</v>
       </c>

</xml_diff>